<commit_message>
Enabled GridOptions on User list (Build 254)
</commit_message>
<xml_diff>
--- a/doc/Planning/Sprint15Plan.xlsx
+++ b/doc/Planning/Sprint15Plan.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="56">
   <si>
     <t>هدف کاری</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>تکمیل امکانات پایه در کنترل گرید</t>
+  </si>
+  <si>
+    <t>سعید قاسمی</t>
   </si>
 </sst>
 </file>
@@ -868,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -969,7 +972,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>49</v>
@@ -988,7 +991,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>49</v>
@@ -1007,7 +1010,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Fixed a bug in assigning users to roles (Build 262)
</commit_message>
<xml_diff>
--- a/doc/Planning/Sprint15Plan.xlsx
+++ b/doc/Planning/Sprint15Plan.xlsx
@@ -872,7 +872,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1050,7 +1050,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>49</v>
@@ -1069,7 +1069,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>49</v>
@@ -1088,7 +1088,7 @@
         <v>1</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>49</v>
@@ -1109,7 +1109,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>49</v>
@@ -1128,7 +1128,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>49</v>

</xml_diff>